<commit_message>
feat: add employee_baseline + month_std, batch scripts for 2023H1/H2 and 2024H1/H2 (wide/narrow), import API month_std fill, and single-employee helpers
</commit_message>
<xml_diff>
--- a/数据/五险一金测算逻辑.xlsx
+++ b/数据/五险一金测算逻辑.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="11630" activeTab="6"/>
+    <workbookView windowWidth="25600" windowHeight="12080" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="解读" sheetId="51" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
     <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="181" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="83">
+  <fonts count="75">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2874,13 +2874,6 @@
       <color indexed="8"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2976,21 +2969,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="等线"/>
@@ -3004,12 +2982,6 @@
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -3034,12 +3006,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -3096,13 +3062,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
@@ -3152,13 +3111,6 @@
       <color rgb="FFC00000"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -3304,12 +3256,38 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -3327,44 +3305,12 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFC00000"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="8"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei UI"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3383,7 +3329,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3494,12 +3440,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3524,18 +3464,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3549,18 +3477,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3602,12 +3518,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3639,18 +3549,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4024,180 +3922,180 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="50" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="17" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="18" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="51" fillId="18" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="19" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="13" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="19" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="13" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="20" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="54" fillId="19" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="63" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="58" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="66" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="59" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="68" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="69" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="62" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4268,10 +4166,10 @@
     <xf numFmtId="177" fontId="6" fillId="3" borderId="1" xfId="59" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="50">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="50">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="6" fillId="0" borderId="1" xfId="59" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4286,128 +4184,128 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="59" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="50" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="50" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="50" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="50" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="1" xfId="59" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="1" xfId="62" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="9" fillId="0" borderId="1" xfId="62" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="50" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="50" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="179" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="13" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="15" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="16" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="11" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4418,19 +4316,19 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="18" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="9" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4439,20 +4337,20 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4467,7 +4365,7 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4476,26 +4374,26 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4507,28 +4405,25 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="24" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="22" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="22" fillId="12" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4540,224 +4435,218 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="61">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="63">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="63">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="61" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="61" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="63" applyFont="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="63" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="61" applyFont="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="61" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="63" applyFont="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="63" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="57" fontId="11" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="57" fontId="10" fillId="0" borderId="0" xfId="61" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="61" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="61" applyFont="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="61" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="53"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="53" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="11" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="11" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="11" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="11" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="13" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="19" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="29" fillId="0" borderId="1" xfId="58" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="1" xfId="58" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="30" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="35" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="36" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="20" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="20" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="14" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="29" fillId="12" borderId="1" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="34" fillId="12" borderId="1" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="30" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="35" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="31" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="36" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="37" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="32" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="37" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="0" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="0" borderId="13" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="0" borderId="13" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="30" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="35" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="32" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="37" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="32" fillId="12" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="37" fillId="12" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="12" borderId="13" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="12" borderId="13" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="30" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="35" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="34" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="39" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="30" fillId="12" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="35" fillId="12" borderId="11" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="13" borderId="12" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="2" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="13" borderId="2" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="30" fillId="10" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="35" fillId="10" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="32" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="41" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="32" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="41" fillId="12" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="30" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="35" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="4" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="4" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="13" borderId="10" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="30" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="35" fillId="0" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="30" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="12" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="35" fillId="12" borderId="1" xfId="55" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="1" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="56" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="15" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="16" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="12" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="55" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="12" borderId="1" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="56" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="56" applyAlignment="1">
+    <xf numFmtId="14" fontId="42" fillId="0" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="15" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="56" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="48" fillId="0" borderId="21" xfId="56" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="56" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="21" xfId="56" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="21" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="21" xfId="56" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4827,17 +4716,7 @@
     <cellStyle name="常规_2月份" xfId="62"/>
     <cellStyle name="超链接 2" xfId="63"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -23171,202 +23050,202 @@
   <dimension ref="B2:I28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="7" width="8.66666666666667" style="193"/>
-    <col min="8" max="8" width="12.9166666666667" style="193" customWidth="1"/>
-    <col min="9" max="9" width="35" style="193" customWidth="1"/>
-    <col min="10" max="16384" width="8.66666666666667" style="193"/>
+    <col min="1" max="7" width="8.66666666666667" style="190"/>
+    <col min="8" max="8" width="12.9166666666667" style="190" customWidth="1"/>
+    <col min="9" max="9" width="35" style="190" customWidth="1"/>
+    <col min="10" max="16384" width="8.66666666666667" style="190"/>
   </cols>
   <sheetData>
     <row r="2" ht="13" spans="2:2">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="191" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" ht="14.5" spans="2:9">
-      <c r="B4" s="195" t="s">
+      <c r="B4" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="195" t="s">
+      <c r="C4" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="195" t="s">
+      <c r="D4" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="195" t="s">
+      <c r="E4" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="195" t="s">
+      <c r="F4" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="196" t="s">
+      <c r="H4" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="196" t="s">
+      <c r="I4" s="193" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="14.5" spans="2:9">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="197"/>
-      <c r="D5" s="197"/>
-      <c r="E5" s="197"/>
-      <c r="F5" s="197"/>
-      <c r="H5" s="198" t="s">
+      <c r="C5" s="194"/>
+      <c r="D5" s="194"/>
+      <c r="E5" s="194"/>
+      <c r="F5" s="194"/>
+      <c r="H5" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="200" t="s">
+      <c r="I5" s="197" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="14.5" spans="2:9">
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="194" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="197"/>
-      <c r="D6" s="197"/>
-      <c r="E6" s="197"/>
-      <c r="F6" s="197"/>
-      <c r="H6" s="198" t="s">
+      <c r="C6" s="194"/>
+      <c r="D6" s="194"/>
+      <c r="E6" s="194"/>
+      <c r="F6" s="194"/>
+      <c r="H6" s="195" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="201" t="s">
+      <c r="I6" s="198" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" ht="14.5" spans="2:9">
-      <c r="B7" s="197" t="s">
+      <c r="B7" s="194" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="197"/>
-      <c r="D7" s="197"/>
-      <c r="E7" s="197"/>
-      <c r="F7" s="197"/>
-      <c r="H7" s="198" t="s">
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
+      <c r="H7" s="195" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="201" t="s">
+      <c r="I7" s="198" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="14.5" spans="2:9">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="194" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="197"/>
-      <c r="D8" s="197"/>
-      <c r="E8" s="197"/>
-      <c r="F8" s="197"/>
-      <c r="H8" s="198" t="s">
+      <c r="C8" s="194"/>
+      <c r="D8" s="194"/>
+      <c r="E8" s="194"/>
+      <c r="F8" s="194"/>
+      <c r="H8" s="195" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="201" t="s">
+      <c r="I8" s="198" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" ht="14.5" spans="2:9">
-      <c r="B9" s="197" t="s">
+      <c r="B9" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="197"/>
-      <c r="D9" s="197"/>
-      <c r="E9" s="197"/>
-      <c r="F9" s="197"/>
-      <c r="H9" s="198" t="s">
+      <c r="C9" s="194"/>
+      <c r="D9" s="194"/>
+      <c r="E9" s="194"/>
+      <c r="F9" s="194"/>
+      <c r="H9" s="195" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="201" t="s">
+      <c r="I9" s="198" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" ht="13" spans="2:6">
-      <c r="B10" s="195" t="s">
+      <c r="B10" s="192" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="195" t="s">
+      <c r="C10" s="192" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="195" t="s">
+      <c r="D10" s="192" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="195" t="s">
+      <c r="E10" s="192" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="195" t="s">
+      <c r="F10" s="192" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="197" t="s">
+      <c r="B11" s="194" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="197"/>
-      <c r="D11" s="197"/>
-      <c r="E11" s="197"/>
-      <c r="F11" s="197"/>
+      <c r="C11" s="194"/>
+      <c r="D11" s="194"/>
+      <c r="E11" s="194"/>
+      <c r="F11" s="194"/>
     </row>
     <row r="13" ht="13" spans="2:2">
-      <c r="B13" s="192" t="s">
+      <c r="B13" s="189" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" ht="13" spans="2:2">
-      <c r="B14" s="192"/>
+      <c r="B14" s="189"/>
     </row>
-    <row r="15" s="192" customFormat="1" ht="13" spans="2:2">
-      <c r="B15" s="192" t="s">
+    <row r="15" s="189" customFormat="1" ht="13" spans="2:2">
+      <c r="B15" s="189" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" ht="13" spans="2:2">
-      <c r="B16" s="192"/>
+      <c r="B16" s="189"/>
     </row>
     <row r="17" ht="14.5" spans="2:9">
-      <c r="B17" s="192" t="s">
+      <c r="B17" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="199"/>
-      <c r="G17" s="199"/>
-      <c r="H17" s="199"/>
-      <c r="I17" s="199"/>
+      <c r="F17" s="196"/>
+      <c r="G17" s="196"/>
+      <c r="H17" s="196"/>
+      <c r="I17" s="196"/>
     </row>
     <row r="18" ht="13" spans="2:2">
-      <c r="B18" s="192"/>
+      <c r="B18" s="189"/>
     </row>
     <row r="19" ht="13" spans="2:2">
-      <c r="B19" s="192" t="s">
+      <c r="B19" s="189" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="22" ht="13" spans="2:2">
-      <c r="B22" s="194" t="s">
+      <c r="B22" s="191" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" ht="13" spans="2:2">
-      <c r="B24" s="192" t="s">
+      <c r="B24" s="189" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" ht="13" spans="2:2">
-      <c r="B25" s="192"/>
+      <c r="B25" s="189"/>
     </row>
     <row r="26" ht="13" spans="2:2">
-      <c r="B26" s="192" t="s">
+      <c r="B26" s="189" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" ht="13" spans="2:2">
-      <c r="B27" s="192"/>
+      <c r="B27" s="189"/>
     </row>
     <row r="28" ht="13" spans="2:2">
-      <c r="B28" s="192" t="s">
+      <c r="B28" s="189" t="s">
         <v>30</v>
       </c>
     </row>
@@ -23385,7 +23264,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -23402,12 +23281,12 @@
   </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:C27"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
@@ -24099,16 +23978,16 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
     <cfRule type="duplicateValues" dxfId="0" priority="948"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1357"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1357"/>
     <cfRule type="duplicateValues" dxfId="0" priority="947"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
     <cfRule type="duplicateValues" dxfId="0" priority="880"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1662"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1662"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
     <cfRule type="duplicateValues" dxfId="0" priority="806"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1933"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1933"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
     <cfRule type="duplicateValues" dxfId="0" priority="726"/>
@@ -24135,7 +24014,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="2" priority="1935"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1935"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -24152,7 +24031,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C27"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" outlineLevelRow="4"/>
@@ -24408,27 +24287,27 @@
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="2" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="2" priority="1941"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1941"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="2" priority="1969"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="1970"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1969"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1970"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="1" priority="1986"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1986"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="2" priority="2019"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2020"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2019"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2020"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:B1048576 B1:B2">
-    <cfRule type="duplicateValues" dxfId="1" priority="2042"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2042"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:I1 K1:O1">
-    <cfRule type="duplicateValues" dxfId="1" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -24445,821 +24324,829 @@
   <dimension ref="B2:AB23"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B2" sqref="B2:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="5" style="141" customWidth="1"/>
-    <col min="2" max="2" width="18.3333333333333" style="141" customWidth="1"/>
-    <col min="3" max="3" width="28.3333333333333" style="141" customWidth="1"/>
-    <col min="4" max="8" width="13" style="141" customWidth="1"/>
-    <col min="9" max="9" width="15.3333333333333" style="141" customWidth="1"/>
-    <col min="10" max="10" width="15.9166666666667" style="141" customWidth="1"/>
-    <col min="11" max="11" width="25.4166666666667" style="141" customWidth="1"/>
-    <col min="12" max="12" width="13" style="141" customWidth="1"/>
-    <col min="13" max="13" width="15.5833333333333" style="141" customWidth="1"/>
-    <col min="14" max="15" width="13" style="141" customWidth="1"/>
-    <col min="16" max="16" width="23.4166666666667" style="141" customWidth="1"/>
-    <col min="17" max="17" width="19.4166666666667" style="141" customWidth="1"/>
-    <col min="18" max="19" width="11.9166666666667" style="141" customWidth="1"/>
-    <col min="20" max="23" width="19.4166666666667" style="141" customWidth="1"/>
-    <col min="24" max="25" width="13" style="141" customWidth="1"/>
-    <col min="26" max="27" width="15" style="141" customWidth="1"/>
-    <col min="28" max="28" width="55.75" style="141" customWidth="1"/>
-    <col min="29" max="16384" width="8.66666666666667" style="141"/>
+    <col min="1" max="1" width="5" style="139" customWidth="1"/>
+    <col min="2" max="2" width="18.3333333333333" style="139" customWidth="1"/>
+    <col min="3" max="3" width="28.3333333333333" style="139" customWidth="1"/>
+    <col min="4" max="4" width="13" style="139" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="139" customWidth="1"/>
+    <col min="6" max="6" width="13" style="139" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="139" customWidth="1"/>
+    <col min="8" max="8" width="13" style="139" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3333333333333" style="139" customWidth="1"/>
+    <col min="10" max="10" width="15.9166666666667" style="139" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7666666666667" style="139" customWidth="1"/>
+    <col min="12" max="12" width="13" style="139" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5833333333333" style="139" customWidth="1"/>
+    <col min="14" max="14" width="13" style="139" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="13" style="139" customWidth="1"/>
+    <col min="16" max="16" width="14.05" style="139" customWidth="1"/>
+    <col min="17" max="17" width="11.95" style="139" customWidth="1"/>
+    <col min="18" max="19" width="11.9166666666667" style="139" customWidth="1"/>
+    <col min="20" max="20" width="11.0083333333333" style="139" customWidth="1"/>
+    <col min="21" max="21" width="11.45" style="139" customWidth="1"/>
+    <col min="22" max="22" width="12.5333333333333" style="139" customWidth="1"/>
+    <col min="23" max="23" width="10.4333333333333" style="139" customWidth="1"/>
+    <col min="24" max="25" width="13" style="139" customWidth="1"/>
+    <col min="26" max="27" width="15" style="139" customWidth="1"/>
+    <col min="28" max="28" width="55.75" style="139" customWidth="1"/>
+    <col min="29" max="16384" width="8.66666666666667" style="139"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
-      <c r="B2" s="142" t="s">
+      <c r="B2" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="143"/>
-      <c r="F2" s="143"/>
-      <c r="G2" s="143"/>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
-      <c r="K2" s="143"/>
-      <c r="L2" s="143"/>
-      <c r="M2" s="143"/>
-      <c r="N2" s="143"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="141"/>
+      <c r="I2" s="141"/>
+      <c r="J2" s="141"/>
+      <c r="K2" s="141"/>
+      <c r="L2" s="141"/>
+      <c r="M2" s="141"/>
+      <c r="N2" s="141"/>
     </row>
     <row r="3" spans="2:14">
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143"/>
+      <c r="B3" s="141"/>
+      <c r="C3" s="141"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
+      <c r="G3" s="141"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="141"/>
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="141"/>
+      <c r="M3" s="141"/>
+      <c r="N3" s="141"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="143"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="143"/>
-      <c r="K4" s="143"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="143"/>
-      <c r="N4" s="143"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="141"/>
+      <c r="I4" s="141"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="141"/>
+      <c r="M4" s="141"/>
+      <c r="N4" s="141"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="143"/>
-      <c r="C5" s="143"/>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
-      <c r="H5" s="143"/>
-      <c r="I5" s="143"/>
-      <c r="J5" s="143"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
-      <c r="N5" s="143"/>
+      <c r="B5" s="141"/>
+      <c r="C5" s="141"/>
+      <c r="D5" s="141"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="141"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="143"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
-      <c r="I6" s="143"/>
-      <c r="J6" s="143"/>
-      <c r="K6" s="143"/>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="143"/>
+      <c r="B6" s="141"/>
+      <c r="C6" s="141"/>
+      <c r="D6" s="141"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="141"/>
+      <c r="G6" s="141"/>
+      <c r="H6" s="141"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="141"/>
+      <c r="N6" s="141"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="143"/>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
-      <c r="E7" s="143"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="143"/>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="143"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="143"/>
-      <c r="C8" s="143"/>
-      <c r="D8" s="143"/>
-      <c r="E8" s="143"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="143"/>
-      <c r="K8" s="143"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="143"/>
-      <c r="N8" s="143"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="141"/>
+      <c r="D8" s="141"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="141"/>
+      <c r="G8" s="141"/>
+      <c r="H8" s="141"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="141"/>
+      <c r="M8" s="141"/>
+      <c r="N8" s="141"/>
     </row>
     <row r="12" spans="2:28">
-      <c r="B12" s="144" t="s">
+      <c r="B12" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="145" t="s">
+      <c r="C12" s="142" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="146" t="s">
+      <c r="D12" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="147"/>
-      <c r="F12" s="148" t="s">
+      <c r="E12" s="144"/>
+      <c r="F12" s="145" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="149"/>
-      <c r="H12" s="148" t="s">
+      <c r="G12" s="146"/>
+      <c r="H12" s="145" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="149"/>
-      <c r="J12" s="148" t="s">
+      <c r="I12" s="146"/>
+      <c r="J12" s="145" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="149"/>
-      <c r="L12" s="148" t="s">
+      <c r="K12" s="146"/>
+      <c r="L12" s="145" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="149"/>
-      <c r="N12" s="148" t="s">
+      <c r="M12" s="146"/>
+      <c r="N12" s="145" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="149"/>
-      <c r="P12" s="146" t="s">
+      <c r="O12" s="146"/>
+      <c r="P12" s="143" t="s">
         <v>40</v>
       </c>
-      <c r="Q12" s="178"/>
-      <c r="R12" s="178"/>
-      <c r="S12" s="178"/>
-      <c r="T12" s="178"/>
-      <c r="U12" s="178"/>
-      <c r="V12" s="178"/>
-      <c r="W12" s="147"/>
-      <c r="X12" s="179" t="s">
+      <c r="Q12" s="175"/>
+      <c r="R12" s="175"/>
+      <c r="S12" s="175"/>
+      <c r="T12" s="175"/>
+      <c r="U12" s="175"/>
+      <c r="V12" s="175"/>
+      <c r="W12" s="144"/>
+      <c r="X12" s="176" t="s">
         <v>41</v>
       </c>
-      <c r="Y12" s="184"/>
-      <c r="Z12" s="144" t="s">
+      <c r="Y12" s="181"/>
+      <c r="Z12" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="AA12" s="185" t="s">
+      <c r="AA12" s="182" t="s">
         <v>43</v>
       </c>
-      <c r="AB12" s="185" t="s">
+      <c r="AB12" s="182" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" ht="25.75" customHeight="1" spans="2:28">
-      <c r="B13" s="150"/>
-      <c r="C13" s="151"/>
-      <c r="D13" s="145" t="s">
+      <c r="B13" s="147"/>
+      <c r="C13" s="148"/>
+      <c r="D13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="152" t="s">
+      <c r="E13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="145" t="s">
+      <c r="F13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="G13" s="152" t="s">
+      <c r="G13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="H13" s="145" t="s">
+      <c r="H13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="152" t="s">
+      <c r="I13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="J13" s="145" t="s">
+      <c r="J13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="152" t="s">
+      <c r="K13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="145" t="s">
+      <c r="L13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="152" t="s">
+      <c r="M13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="N13" s="145" t="s">
+      <c r="N13" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="152" t="s">
+      <c r="O13" s="149" t="s">
         <v>46</v>
       </c>
-      <c r="P13" s="164" t="s">
+      <c r="P13" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="164" t="s">
+      <c r="Q13" s="161" t="s">
         <v>48</v>
       </c>
-      <c r="R13" s="164" t="s">
+      <c r="R13" s="161" t="s">
         <v>49</v>
       </c>
-      <c r="S13" s="164" t="s">
+      <c r="S13" s="161" t="s">
         <v>50</v>
       </c>
-      <c r="T13" s="164" t="s">
+      <c r="T13" s="161" t="s">
         <v>51</v>
       </c>
-      <c r="U13" s="164" t="s">
+      <c r="U13" s="161" t="s">
         <v>52</v>
       </c>
-      <c r="V13" s="164" t="s">
+      <c r="V13" s="161" t="s">
         <v>53</v>
       </c>
-      <c r="W13" s="164" t="s">
+      <c r="W13" s="161" t="s">
         <v>54</v>
       </c>
-      <c r="X13" s="164" t="s">
+      <c r="X13" s="161" t="s">
         <v>55</v>
       </c>
-      <c r="Y13" s="164" t="s">
+      <c r="Y13" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="Z13" s="151"/>
-      <c r="AA13" s="151"/>
-      <c r="AB13" s="151"/>
+      <c r="Z13" s="148"/>
+      <c r="AA13" s="148"/>
+      <c r="AB13" s="148"/>
     </row>
-    <row r="14" ht="45" spans="2:28">
-      <c r="B14" s="144" t="s">
+    <row r="14" ht="45" hidden="1" spans="2:28">
+      <c r="B14" s="142" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="152" t="s">
+      <c r="C14" s="149" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="153">
+      <c r="D14" s="150">
         <v>0.08</v>
       </c>
-      <c r="E14" s="154">
+      <c r="E14" s="151">
         <v>0.14</v>
       </c>
-      <c r="F14" s="155">
+      <c r="F14" s="152">
         <v>0</v>
       </c>
-      <c r="G14" s="156" t="s">
+      <c r="G14" s="153" t="s">
         <v>59</v>
       </c>
-      <c r="H14" s="154">
+      <c r="H14" s="151">
         <v>0.002</v>
       </c>
-      <c r="I14" s="165" t="s">
+      <c r="I14" s="162" t="s">
         <v>60</v>
       </c>
-      <c r="J14" s="166" t="s">
+      <c r="J14" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="167">
+      <c r="K14" s="164">
         <v>0.03</v>
       </c>
-      <c r="L14" s="154">
+      <c r="L14" s="151">
         <v>0</v>
       </c>
-      <c r="M14" s="154" t="s">
+      <c r="M14" s="151" t="s">
         <v>62</v>
       </c>
-      <c r="N14" s="168" t="s">
+      <c r="N14" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="O14" s="168" t="s">
+      <c r="O14" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="P14" s="169">
+      <c r="P14" s="166">
         <v>3958</v>
       </c>
-      <c r="Q14" s="169">
+      <c r="Q14" s="166">
         <v>22941</v>
       </c>
-      <c r="R14" s="169"/>
-      <c r="S14" s="169"/>
-      <c r="T14" s="169">
+      <c r="R14" s="166"/>
+      <c r="S14" s="166"/>
+      <c r="T14" s="166">
         <v>1720</v>
       </c>
-      <c r="U14" s="169">
+      <c r="U14" s="166">
         <v>23634</v>
       </c>
-      <c r="V14" s="180">
+      <c r="V14" s="177">
         <v>5626</v>
       </c>
-      <c r="W14" s="180">
+      <c r="W14" s="177">
         <v>5626</v>
       </c>
-      <c r="X14" s="181">
+      <c r="X14" s="178">
         <v>1900</v>
       </c>
-      <c r="Y14" s="169">
+      <c r="Y14" s="166">
         <v>23634</v>
       </c>
-      <c r="Z14" s="186"/>
-      <c r="AA14" s="154"/>
-      <c r="AB14" s="187" t="s">
+      <c r="Z14" s="183"/>
+      <c r="AA14" s="151"/>
+      <c r="AB14" s="184" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" ht="61.25" customHeight="1" spans="2:28">
-      <c r="B15" s="157"/>
-      <c r="C15" s="152" t="s">
+    <row r="15" ht="61.25" hidden="1" customHeight="1" spans="2:28">
+      <c r="B15" s="154"/>
+      <c r="C15" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="153">
+      <c r="D15" s="150">
         <v>0.08</v>
       </c>
-      <c r="E15" s="154">
+      <c r="E15" s="151">
         <v>0.14</v>
       </c>
-      <c r="F15" s="155">
+      <c r="F15" s="152">
         <v>0</v>
       </c>
-      <c r="G15" s="158" t="s">
+      <c r="G15" s="155" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="154">
+      <c r="H15" s="151">
         <v>0.002</v>
       </c>
-      <c r="I15" s="165" t="s">
+      <c r="I15" s="162" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="166" t="s">
+      <c r="J15" s="163" t="s">
         <v>61</v>
       </c>
-      <c r="K15" s="167">
+      <c r="K15" s="164">
         <v>0.035</v>
       </c>
-      <c r="L15" s="154">
+      <c r="L15" s="151">
         <v>0</v>
       </c>
-      <c r="M15" s="154" t="s">
+      <c r="M15" s="151" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="168" t="s">
+      <c r="N15" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="168" t="s">
+      <c r="O15" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="169">
+      <c r="P15" s="166">
         <v>3958</v>
       </c>
-      <c r="Q15" s="169">
+      <c r="Q15" s="166">
         <v>22941</v>
       </c>
-      <c r="R15" s="169"/>
-      <c r="S15" s="169"/>
-      <c r="T15" s="169">
+      <c r="R15" s="166"/>
+      <c r="S15" s="166"/>
+      <c r="T15" s="166">
         <v>1720</v>
       </c>
-      <c r="U15" s="169">
+      <c r="U15" s="166">
         <v>23634</v>
       </c>
-      <c r="V15" s="180">
+      <c r="V15" s="177">
         <v>5626</v>
       </c>
-      <c r="W15" s="180">
+      <c r="W15" s="177">
         <v>5626</v>
       </c>
-      <c r="X15" s="181">
+      <c r="X15" s="178">
         <v>1900</v>
       </c>
-      <c r="Y15" s="169">
+      <c r="Y15" s="166">
         <v>26070</v>
       </c>
-      <c r="Z15" s="186"/>
-      <c r="AA15" s="154"/>
-      <c r="AB15" s="187" t="s">
+      <c r="Z15" s="183"/>
+      <c r="AA15" s="151"/>
+      <c r="AB15" s="184" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="16" ht="24" customHeight="1" spans="2:28">
-      <c r="B16" s="157"/>
-      <c r="C16" s="159" t="s">
+      <c r="B16" s="154"/>
+      <c r="C16" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="160">
+      <c r="D16" s="157">
         <f>D15</f>
         <v>0.08</v>
       </c>
-      <c r="E16" s="161">
+      <c r="E16" s="158">
         <f>E15</f>
         <v>0.14</v>
       </c>
-      <c r="F16" s="162">
+      <c r="F16" s="159">
         <f>F15</f>
         <v>0</v>
       </c>
-      <c r="G16" s="161">
+      <c r="G16" s="158">
         <v>0.001</v>
       </c>
-      <c r="H16" s="161">
+      <c r="H16" s="158">
         <f>H15</f>
         <v>0.002</v>
       </c>
-      <c r="I16" s="170">
+      <c r="I16" s="167">
         <v>0.0032</v>
       </c>
-      <c r="J16" s="171">
+      <c r="J16" s="168">
         <v>0.02</v>
       </c>
-      <c r="K16" s="161">
+      <c r="K16" s="158">
         <v>0.045</v>
       </c>
-      <c r="L16" s="161">
+      <c r="L16" s="158">
         <f>L15</f>
         <v>0</v>
       </c>
-      <c r="M16" s="161">
+      <c r="M16" s="158">
         <v>0.01</v>
       </c>
-      <c r="N16" s="172">
+      <c r="N16" s="169">
         <v>0.05</v>
       </c>
-      <c r="O16" s="172">
+      <c r="O16" s="169">
         <v>0.05</v>
       </c>
-      <c r="P16" s="173">
+      <c r="P16" s="170">
         <f>P15</f>
         <v>3958</v>
       </c>
-      <c r="Q16" s="173">
+      <c r="Q16" s="170">
         <f>Q15</f>
         <v>22941</v>
       </c>
-      <c r="R16" s="182" t="s">
+      <c r="R16" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="S16" s="182" t="s">
+      <c r="S16" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="T16" s="173">
+      <c r="T16" s="170">
         <f t="shared" ref="T16:Y16" si="0">T15</f>
         <v>1720</v>
       </c>
-      <c r="U16" s="173">
+      <c r="U16" s="170">
         <f t="shared" si="0"/>
         <v>23634</v>
       </c>
-      <c r="V16" s="180">
+      <c r="V16" s="177">
         <f t="shared" si="0"/>
         <v>5626</v>
       </c>
-      <c r="W16" s="180">
+      <c r="W16" s="177">
         <f t="shared" si="0"/>
         <v>5626</v>
       </c>
-      <c r="X16" s="173">
+      <c r="X16" s="170">
         <f t="shared" si="0"/>
         <v>1900</v>
       </c>
-      <c r="Y16" s="173">
+      <c r="Y16" s="170">
         <f t="shared" si="0"/>
         <v>26070</v>
       </c>
-      <c r="Z16" s="188"/>
-      <c r="AA16" s="161"/>
-      <c r="AB16" s="189"/>
+      <c r="Z16" s="185"/>
+      <c r="AA16" s="158"/>
+      <c r="AB16" s="186"/>
     </row>
-    <row r="17" ht="63.65" customHeight="1" spans="2:28">
-      <c r="B17" s="157"/>
-      <c r="C17" s="152" t="s">
+    <row r="17" ht="63.65" hidden="1" customHeight="1" spans="2:28">
+      <c r="B17" s="154"/>
+      <c r="C17" s="149" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="153">
+      <c r="D17" s="150">
         <v>0.08</v>
       </c>
-      <c r="E17" s="154">
+      <c r="E17" s="151">
         <v>0.14</v>
       </c>
-      <c r="F17" s="155">
+      <c r="F17" s="152">
         <v>0</v>
       </c>
-      <c r="G17" s="158" t="s">
+      <c r="G17" s="155" t="s">
         <v>69</v>
       </c>
-      <c r="H17" s="158">
+      <c r="H17" s="155">
         <v>0.002</v>
       </c>
-      <c r="I17" s="158">
+      <c r="I17" s="155">
         <v>0.008</v>
       </c>
-      <c r="J17" s="154" t="s">
+      <c r="J17" s="151" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="174" t="s">
+      <c r="K17" s="171" t="s">
         <v>71</v>
       </c>
-      <c r="L17" s="154">
+      <c r="L17" s="151">
         <v>0</v>
       </c>
-      <c r="M17" s="154" t="s">
+      <c r="M17" s="151" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="168" t="s">
+      <c r="N17" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="O17" s="168" t="s">
+      <c r="O17" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="P17" s="169">
+      <c r="P17" s="166">
         <v>4546</v>
       </c>
-      <c r="Q17" s="169">
+      <c r="Q17" s="166">
         <v>26421</v>
       </c>
-      <c r="R17" s="169"/>
-      <c r="S17" s="169"/>
-      <c r="T17" s="169">
+      <c r="R17" s="166"/>
+      <c r="S17" s="166"/>
+      <c r="T17" s="166">
         <v>1900</v>
       </c>
-      <c r="U17" s="169">
+      <c r="U17" s="166">
         <v>27234</v>
       </c>
-      <c r="V17" s="169">
+      <c r="V17" s="166">
         <v>4340</v>
       </c>
-      <c r="W17" s="169">
+      <c r="W17" s="166">
         <v>21699</v>
       </c>
-      <c r="X17" s="183">
+      <c r="X17" s="180">
         <v>1900</v>
       </c>
-      <c r="Y17" s="169">
+      <c r="Y17" s="166">
         <v>27234</v>
       </c>
-      <c r="Z17" s="186"/>
-      <c r="AA17" s="154"/>
-      <c r="AB17" s="190"/>
+      <c r="Z17" s="183"/>
+      <c r="AA17" s="151"/>
+      <c r="AB17" s="187"/>
     </row>
     <row r="18" ht="15" spans="2:28">
-      <c r="B18" s="157"/>
-      <c r="C18" s="159" t="s">
+      <c r="B18" s="154"/>
+      <c r="C18" s="156" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="160">
+      <c r="D18" s="157">
         <f>D17</f>
         <v>0.08</v>
       </c>
-      <c r="E18" s="160">
+      <c r="E18" s="157">
         <f>E17</f>
         <v>0.14</v>
       </c>
-      <c r="F18" s="160">
+      <c r="F18" s="157">
         <f>F17</f>
         <v>0</v>
       </c>
-      <c r="G18" s="161">
+      <c r="G18" s="158">
         <v>0.0016</v>
       </c>
-      <c r="H18" s="161">
+      <c r="H18" s="158">
         <f>H17</f>
         <v>0.002</v>
       </c>
-      <c r="I18" s="161">
+      <c r="I18" s="158">
         <f>I17</f>
         <v>0.008</v>
       </c>
-      <c r="J18" s="161">
+      <c r="J18" s="158">
         <v>0.02</v>
       </c>
-      <c r="K18" s="161">
+      <c r="K18" s="158">
         <v>0.045</v>
       </c>
-      <c r="L18" s="161">
+      <c r="L18" s="158">
         <f>L17</f>
         <v>0</v>
       </c>
-      <c r="M18" s="161">
+      <c r="M18" s="158">
         <v>0.01</v>
       </c>
-      <c r="N18" s="172">
+      <c r="N18" s="169">
         <v>0.05</v>
       </c>
-      <c r="O18" s="172">
+      <c r="O18" s="169">
         <v>0.05</v>
       </c>
-      <c r="P18" s="175">
+      <c r="P18" s="172">
         <f>P17</f>
         <v>4546</v>
       </c>
-      <c r="Q18" s="175">
+      <c r="Q18" s="172">
         <f>Q17</f>
         <v>26421</v>
       </c>
-      <c r="R18" s="182" t="s">
+      <c r="R18" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="S18" s="182" t="s">
+      <c r="S18" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="T18" s="175">
+      <c r="T18" s="172">
         <f t="shared" ref="T18:Y18" si="1">T17</f>
         <v>1900</v>
       </c>
-      <c r="U18" s="175">
+      <c r="U18" s="172">
         <f t="shared" si="1"/>
         <v>27234</v>
       </c>
-      <c r="V18" s="175">
+      <c r="V18" s="172">
         <f t="shared" si="1"/>
         <v>4340</v>
       </c>
-      <c r="W18" s="175">
+      <c r="W18" s="172">
         <f t="shared" si="1"/>
         <v>21699</v>
       </c>
-      <c r="X18" s="175">
+      <c r="X18" s="172">
         <f t="shared" si="1"/>
         <v>1900</v>
       </c>
-      <c r="Y18" s="175">
+      <c r="Y18" s="172">
         <f t="shared" si="1"/>
         <v>27234</v>
       </c>
-      <c r="Z18" s="188"/>
-      <c r="AA18" s="161"/>
-      <c r="AB18" s="191"/>
+      <c r="Z18" s="185"/>
+      <c r="AA18" s="158"/>
+      <c r="AB18" s="188"/>
     </row>
-    <row r="19" ht="66" customHeight="1" spans="2:28">
-      <c r="B19" s="157"/>
-      <c r="C19" s="152" t="s">
+    <row r="19" ht="66" hidden="1" customHeight="1" spans="2:28">
+      <c r="B19" s="154"/>
+      <c r="C19" s="149" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="153">
+      <c r="D19" s="150">
         <v>0.08</v>
       </c>
-      <c r="E19" s="163">
+      <c r="E19" s="160">
         <v>0.15</v>
       </c>
-      <c r="F19" s="155">
+      <c r="F19" s="152">
         <v>0</v>
       </c>
-      <c r="G19" s="158" t="s">
+      <c r="G19" s="155" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="154">
+      <c r="H19" s="151">
         <v>0.002</v>
       </c>
-      <c r="I19" s="154">
+      <c r="I19" s="151">
         <v>0.008</v>
       </c>
-      <c r="J19" s="154" t="s">
+      <c r="J19" s="151" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="176" t="s">
+      <c r="K19" s="173" t="s">
         <v>75</v>
       </c>
-      <c r="L19" s="154">
+      <c r="L19" s="151">
         <v>0</v>
       </c>
-      <c r="M19" s="154" t="s">
+      <c r="M19" s="151" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="168" t="s">
+      <c r="N19" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="O19" s="168" t="s">
+      <c r="O19" s="165" t="s">
         <v>63</v>
       </c>
-      <c r="P19" s="169">
+      <c r="P19" s="166">
         <v>4546</v>
       </c>
-      <c r="Q19" s="169">
+      <c r="Q19" s="166">
         <v>26421</v>
       </c>
-      <c r="R19" s="169"/>
-      <c r="S19" s="169"/>
-      <c r="T19" s="169">
+      <c r="R19" s="166"/>
+      <c r="S19" s="166"/>
+      <c r="T19" s="166">
         <v>1900</v>
       </c>
-      <c r="U19" s="169">
+      <c r="U19" s="166">
         <v>27234</v>
       </c>
-      <c r="V19" s="169">
+      <c r="V19" s="166">
         <v>4340</v>
       </c>
-      <c r="W19" s="169">
+      <c r="W19" s="166">
         <v>5626</v>
       </c>
-      <c r="X19" s="169">
+      <c r="X19" s="166">
         <v>1900</v>
       </c>
-      <c r="Y19" s="169">
+      <c r="Y19" s="166">
         <v>28770</v>
       </c>
-      <c r="Z19" s="186"/>
-      <c r="AA19" s="154"/>
-      <c r="AB19" s="190"/>
+      <c r="Z19" s="183"/>
+      <c r="AA19" s="151"/>
+      <c r="AB19" s="187"/>
     </row>
     <row r="20" ht="15" spans="2:28">
-      <c r="B20" s="150"/>
-      <c r="C20" s="159" t="s">
+      <c r="B20" s="147"/>
+      <c r="C20" s="156" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="160">
+      <c r="D20" s="157">
         <f>D19</f>
         <v>0.08</v>
       </c>
-      <c r="E20" s="160">
+      <c r="E20" s="157">
         <f>E19</f>
         <v>0.15</v>
       </c>
-      <c r="F20" s="160">
+      <c r="F20" s="157">
         <f>F19</f>
         <v>0</v>
       </c>
-      <c r="G20" s="161">
+      <c r="G20" s="158">
         <v>0.002</v>
       </c>
-      <c r="H20" s="161">
+      <c r="H20" s="158">
         <f>H19</f>
         <v>0.002</v>
       </c>
-      <c r="I20" s="161">
+      <c r="I20" s="158">
         <f>I19</f>
         <v>0.008</v>
       </c>
-      <c r="J20" s="177">
+      <c r="J20" s="174">
         <v>0.02</v>
       </c>
-      <c r="K20" s="177">
+      <c r="K20" s="174">
         <v>0.04</v>
       </c>
-      <c r="L20" s="161">
+      <c r="L20" s="158">
         <f>L19</f>
         <v>0</v>
       </c>
-      <c r="M20" s="161">
+      <c r="M20" s="158">
         <v>0.01</v>
       </c>
-      <c r="N20" s="172">
+      <c r="N20" s="169">
         <v>0.05</v>
       </c>
-      <c r="O20" s="172">
+      <c r="O20" s="169">
         <v>0.05</v>
       </c>
-      <c r="P20" s="173">
+      <c r="P20" s="170">
         <f>P19</f>
         <v>4546</v>
       </c>
-      <c r="Q20" s="173">
+      <c r="Q20" s="170">
         <f>Q19</f>
         <v>26421</v>
       </c>
-      <c r="R20" s="182" t="s">
+      <c r="R20" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="S20" s="182" t="s">
+      <c r="S20" s="179" t="s">
         <v>67</v>
       </c>
-      <c r="T20" s="173">
+      <c r="T20" s="170">
         <f t="shared" ref="T20:Y20" si="2">T19</f>
         <v>1900</v>
       </c>
-      <c r="U20" s="173">
+      <c r="U20" s="170">
         <f t="shared" si="2"/>
         <v>27234</v>
       </c>
-      <c r="V20" s="173">
+      <c r="V20" s="170">
         <f t="shared" si="2"/>
         <v>4340</v>
       </c>
-      <c r="W20" s="173">
+      <c r="W20" s="170">
         <f t="shared" si="2"/>
         <v>5626</v>
       </c>
-      <c r="X20" s="173">
+      <c r="X20" s="170">
         <f t="shared" si="2"/>
         <v>1900</v>
       </c>
-      <c r="Y20" s="173">
+      <c r="Y20" s="170">
         <f t="shared" si="2"/>
         <v>28770</v>
       </c>
-      <c r="Z20" s="188"/>
-      <c r="AA20" s="161"/>
-      <c r="AB20" s="191"/>
+      <c r="Z20" s="185"/>
+      <c r="AA20" s="158"/>
+      <c r="AB20" s="188"/>
     </row>
     <row r="21" ht="20.4" customHeight="1"/>
     <row r="22" ht="20.4" customHeight="1"/>
@@ -25295,131 +25182,131 @@
   <dimension ref="B1:L99"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.91666666666667" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.91666666666667" style="129"/>
-    <col min="2" max="2" width="11.25" style="129" customWidth="1"/>
-    <col min="3" max="11" width="8.91666666666667" style="129"/>
-    <col min="12" max="12" width="12.4166666666667" style="129" customWidth="1"/>
-    <col min="13" max="16384" width="8.91666666666667" style="129"/>
+    <col min="1" max="1" width="8.91666666666667" style="128"/>
+    <col min="2" max="2" width="11.25" style="128" customWidth="1"/>
+    <col min="3" max="11" width="8.91666666666667" style="128"/>
+    <col min="12" max="12" width="12.4166666666667" style="128" customWidth="1"/>
+    <col min="13" max="16384" width="8.91666666666667" style="128"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="136">
+      <c r="B1" s="135">
         <v>44378</v>
       </c>
-      <c r="L1" s="136">
+      <c r="L1" s="135">
         <v>44531</v>
       </c>
     </row>
     <row r="2" spans="2:12">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="132" t="s">
+      <c r="L2" s="131" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="75" spans="2:3">
-      <c r="B75" s="129">
+      <c r="B75" s="128">
         <v>1</v>
       </c>
-      <c r="C75" s="137" t="s">
+      <c r="C75" s="130" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="76" spans="3:3">
-      <c r="C76" s="132" t="s">
+      <c r="C76" s="131" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="78" spans="2:3">
-      <c r="B78" s="129">
+      <c r="B78" s="128">
         <v>2</v>
       </c>
-      <c r="C78" s="129" t="s">
+      <c r="C78" s="128" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="80" spans="3:3">
-      <c r="C80" s="137" t="s">
+      <c r="C80" s="130" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="81" spans="3:3">
-      <c r="C81" s="137" t="s">
+      <c r="C81" s="130" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="83" spans="3:3">
-      <c r="C83" s="132" t="s">
+      <c r="C83" s="131" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="84" spans="3:3">
-      <c r="C84" s="132" t="s">
+      <c r="C84" s="131" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="87" spans="3:3">
-      <c r="C87" s="132" t="s">
+      <c r="C87" s="131" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="88" spans="2:3">
-      <c r="B88" s="129">
+      <c r="B88" s="128">
         <v>3</v>
       </c>
-      <c r="C88" s="129" t="s">
+      <c r="C88" s="128" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:3">
-      <c r="B90" s="138" t="s">
+      <c r="B90" s="136" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="129" t="s">
+      <c r="C90" s="128" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="91" spans="2:3">
-      <c r="B91" s="138"/>
-      <c r="C91" s="128" t="s">
+      <c r="B91" s="136"/>
+      <c r="C91" s="127" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="92" spans="2:3">
-      <c r="B92" s="138" t="s">
+      <c r="B92" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="C92" s="129" t="s">
+      <c r="C92" s="128" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="93" spans="2:3">
-      <c r="B93" s="138"/>
-      <c r="C93" s="132" t="s">
+      <c r="B93" s="136"/>
+      <c r="C93" s="131" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="96" spans="2:3">
-      <c r="B96" s="129">
+      <c r="B96" s="128">
         <v>4</v>
       </c>
-      <c r="C96" s="139" t="s">
+      <c r="C96" s="137" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="97" spans="3:3">
-      <c r="C97" s="129" t="s">
+      <c r="C97" s="128" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="99" spans="3:3">
-      <c r="C99" s="140" t="s">
+      <c r="C99" s="138" t="s">
         <v>95</v>
       </c>
     </row>
@@ -25446,61 +25333,61 @@
   <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.91666666666667" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.91666666666667" style="127"/>
+    <col min="1" max="16384" width="8.91666666666667" style="126"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="127" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="11:12">
-      <c r="K4" s="127">
+      <c r="K4" s="126">
         <v>1</v>
       </c>
-      <c r="L4" s="133" t="s">
+      <c r="L4" s="132" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="12:12">
-      <c r="L5" s="134"/>
+      <c r="L5" s="133"/>
     </row>
     <row r="6" spans="12:12">
-      <c r="L6" s="133" t="s">
+      <c r="L6" s="132" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="7" spans="12:12">
-      <c r="L7" s="134"/>
+      <c r="L7" s="133"/>
     </row>
     <row r="8" spans="12:12">
-      <c r="L8" s="135" t="s">
+      <c r="L8" s="134" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="12:12">
-      <c r="L9" s="134"/>
+      <c r="L9" s="133"/>
     </row>
     <row r="10" spans="12:12">
-      <c r="L10" s="135" t="s">
+      <c r="L10" s="134" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="14" spans="11:12">
-      <c r="K14" s="127">
+      <c r="K14" s="126">
         <v>2</v>
       </c>
-      <c r="L14" s="127" t="s">
+      <c r="L14" s="126" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="12:12">
-      <c r="L15" s="127" t="s">
+      <c r="L15" s="126" t="s">
         <v>101</v>
       </c>
     </row>
@@ -25522,82 +25409,82 @@
   <dimension ref="B2:C24"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.91666666666667" defaultRowHeight="14" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="2.58333333333333" style="129" customWidth="1"/>
-    <col min="2" max="2" width="6.58333333333333" style="130" customWidth="1"/>
-    <col min="3" max="3" width="146.25" style="129" customWidth="1"/>
-    <col min="4" max="16384" width="8.91666666666667" style="129"/>
+    <col min="1" max="1" width="2.58333333333333" style="128" customWidth="1"/>
+    <col min="2" max="2" width="6.58333333333333" style="129" customWidth="1"/>
+    <col min="3" max="3" width="146.25" style="128" customWidth="1"/>
+    <col min="4" max="16384" width="8.91666666666667" style="128"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="130">
+      <c r="B2" s="129">
         <v>1</v>
       </c>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="130" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="3:3">
-      <c r="C4" s="132" t="s">
+      <c r="C4" s="131" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="3:3">
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="131" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="7" ht="286.75" customHeight="1"/>
     <row r="9" ht="16.5" spans="2:3">
-      <c r="B9" s="130">
+      <c r="B9" s="129">
         <v>2</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="130" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="3:3">
-      <c r="C11" s="132" t="s">
+      <c r="C11" s="131" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="13" spans="2:3">
-      <c r="B13" s="130">
+      <c r="B13" s="129">
         <v>3</v>
       </c>
-      <c r="C13" s="129" t="s">
+      <c r="C13" s="128" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="15" spans="3:3">
-      <c r="C15" s="129" t="s">
+      <c r="C15" s="128" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="17" spans="3:3">
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="131" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" ht="16.5" spans="2:3">
-      <c r="B19" s="130">
+      <c r="B19" s="129">
         <v>4</v>
       </c>
-      <c r="C19" s="129" t="s">
+      <c r="C19" s="128" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="3:3">
-      <c r="C20" s="129" t="s">
+      <c r="C20" s="128" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="24" spans="3:3">
-      <c r="C24" s="128" t="s">
+      <c r="C24" s="127" t="s">
         <v>111</v>
       </c>
     </row>
@@ -25621,45 +25508,45 @@
   <dimension ref="B2:L60"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.91666666666667" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="8.91666666666667" style="127"/>
+    <col min="1" max="16384" width="8.91666666666667" style="126"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="K2" s="127">
+      <c r="K2" s="126">
         <v>1</v>
       </c>
-      <c r="L2" s="127" t="s">
+      <c r="L2" s="126" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="25" spans="12:12">
-      <c r="L25" s="128" t="s">
+      <c r="L25" s="127" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="42" spans="12:12">
-      <c r="L42" s="128" t="s">
+      <c r="L42" s="127" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="59" spans="11:12">
-      <c r="K59" s="127">
+      <c r="K59" s="126">
         <v>2</v>
       </c>
-      <c r="L59" s="127" t="s">
+      <c r="L59" s="126" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="60" spans="12:12">
-      <c r="L60" s="127" t="s">
+      <c r="L60" s="126" t="s">
         <v>117</v>
       </c>
     </row>
@@ -25682,7 +25569,7 @@
   </sheetPr>
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -25791,13 +25678,13 @@
       <c r="AF2" s="116"/>
       <c r="AG2" s="116"/>
       <c r="AH2" s="116"/>
-      <c r="AI2" s="125" t="s">
+      <c r="AI2" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="AJ2" s="125"/>
-      <c r="AK2" s="125"/>
-      <c r="AL2" s="125"/>
-      <c r="AM2" s="125"/>
+      <c r="AJ2" s="124"/>
+      <c r="AK2" s="124"/>
+      <c r="AL2" s="124"/>
+      <c r="AM2" s="124"/>
     </row>
     <row r="3" ht="42" spans="2:39">
       <c r="B3" s="88" t="s">
@@ -25860,7 +25747,7 @@
       <c r="U3" s="118" t="s">
         <v>135</v>
       </c>
-      <c r="V3" s="119" t="s">
+      <c r="V3" s="118" t="s">
         <v>136</v>
       </c>
       <c r="W3" s="116" t="s">
@@ -25869,13 +25756,13 @@
       <c r="X3" s="118" t="s">
         <v>138</v>
       </c>
-      <c r="Y3" s="119" t="s">
+      <c r="Y3" s="118" t="s">
         <v>139</v>
       </c>
       <c r="Z3" s="116" t="s">
         <v>140</v>
       </c>
-      <c r="AA3" s="119" t="s">
+      <c r="AA3" s="118" t="s">
         <v>141</v>
       </c>
       <c r="AB3" s="116" t="s">
@@ -25890,28 +25777,28 @@
       <c r="AE3" s="116" t="s">
         <v>145</v>
       </c>
-      <c r="AF3" s="123" t="s">
+      <c r="AF3" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="AG3" s="123" t="s">
+      <c r="AG3" s="122" t="s">
         <v>147</v>
       </c>
       <c r="AH3" s="116" t="s">
         <v>148</v>
       </c>
-      <c r="AI3" s="125" t="s">
+      <c r="AI3" s="124" t="s">
         <v>137</v>
       </c>
-      <c r="AJ3" s="125" t="s">
+      <c r="AJ3" s="124" t="s">
         <v>140</v>
       </c>
-      <c r="AK3" s="125" t="s">
+      <c r="AK3" s="124" t="s">
         <v>142</v>
       </c>
-      <c r="AL3" s="125" t="s">
+      <c r="AL3" s="124" t="s">
         <v>145</v>
       </c>
-      <c r="AM3" s="125" t="s">
+      <c r="AM3" s="124" t="s">
         <v>148</v>
       </c>
     </row>
@@ -25936,65 +25823,65 @@
       <c r="Q4" s="111"/>
       <c r="R4" s="111"/>
       <c r="S4" s="111"/>
-      <c r="T4" s="120"/>
-      <c r="U4" s="121">
+      <c r="T4" s="119"/>
+      <c r="U4" s="120">
         <f>五险一金比例基数示意!P18</f>
         <v>4546</v>
       </c>
-      <c r="V4" s="121">
+      <c r="V4" s="120">
         <f>五险一金比例基数示意!Q18</f>
         <v>26421</v>
       </c>
-      <c r="W4" s="122">
+      <c r="W4" s="121">
         <f>五险一金比例基数示意!E18</f>
         <v>0.14</v>
       </c>
-      <c r="X4" s="121">
+      <c r="X4" s="120">
         <f>五险一金比例基数示意!T18</f>
         <v>1900</v>
       </c>
-      <c r="Y4" s="121">
+      <c r="Y4" s="120">
         <f>五险一金比例基数示意!U18</f>
         <v>27234</v>
       </c>
-      <c r="Z4" s="122">
+      <c r="Z4" s="121">
         <f>五险一金比例基数示意!I18</f>
         <v>0.008</v>
       </c>
-      <c r="AA4" s="122"/>
-      <c r="AB4" s="122">
+      <c r="AA4" s="121"/>
+      <c r="AB4" s="121">
         <f>五险一金比例基数示意!G18</f>
         <v>0.0016</v>
       </c>
-      <c r="AC4" s="121">
+      <c r="AC4" s="120">
         <f>五险一金比例基数示意!V18</f>
         <v>4340</v>
       </c>
-      <c r="AD4" s="121">
+      <c r="AD4" s="120">
         <f>五险一金比例基数示意!W18</f>
         <v>21699</v>
       </c>
-      <c r="AE4" s="122">
+      <c r="AE4" s="121">
         <f>五险一金比例基数示意!K18</f>
         <v>0.045</v>
       </c>
-      <c r="AF4" s="124">
+      <c r="AF4" s="123">
         <f>五险一金比例基数示意!X18</f>
         <v>1900</v>
       </c>
-      <c r="AG4" s="124">
+      <c r="AG4" s="123">
         <f>五险一金比例基数示意!Y18</f>
         <v>27234</v>
       </c>
-      <c r="AH4" s="122">
+      <c r="AH4" s="121">
         <f>五险一金比例基数示意!O18</f>
         <v>0.05</v>
       </c>
-      <c r="AI4" s="126"/>
-      <c r="AJ4" s="126"/>
-      <c r="AK4" s="126"/>
-      <c r="AL4" s="126"/>
-      <c r="AM4" s="126"/>
+      <c r="AI4" s="125"/>
+      <c r="AJ4" s="125"/>
+      <c r="AK4" s="125"/>
+      <c r="AL4" s="125"/>
+      <c r="AM4" s="125"/>
     </row>
     <row r="5" s="81" customFormat="1" spans="1:39">
       <c r="A5" s="81" t="s">
@@ -26272,7 +26159,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.83333333333333" defaultRowHeight="14"/>
@@ -27053,7 +26940,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>

</xml_diff>